<commit_message>
update flash layout doc
</commit_message>
<xml_diff>
--- a/testmyself3152/DOC/flash分配.xlsx
+++ b/testmyself3152/DOC/flash分配.xlsx
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -557,7 +557,7 @@
     <col min="6" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -574,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -590,8 +590,11 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2">
+        <v>12032</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -608,7 +611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -625,7 +628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -642,7 +645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -657,7 +660,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -674,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -691,7 +694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -706,6 +709,9 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="F9" s="2">
+        <v>12160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lux control CODE is tested
</commit_message>
<xml_diff>
--- a/testmyself3152/DOC/flash分配.xlsx
+++ b/testmyself3152/DOC/flash分配.xlsx
@@ -94,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SWITCHfXBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x2F07</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,6 +135,10 @@
   </si>
   <si>
     <t>不开雷达时的亮度值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work_mode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,7 +544,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -605,7 +605,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -622,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -639,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -671,7 +671,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
@@ -682,16 +682,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -699,16 +699,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="2">
         <v>12160</v>

</xml_diff>

<commit_message>
fix the work_mode initial value
</commit_message>
<xml_diff>
--- a/testmyself3152/DOC/flash分配.xlsx
+++ b/testmyself3152/DOC/flash分配.xlsx
@@ -114,10 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>雷达开关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>关灯延时</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,6 +135,10 @@
   </si>
   <si>
     <t>work_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块工作模式</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,7 +544,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -622,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -671,7 +671,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
@@ -682,13 +682,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
@@ -705,7 +705,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>

</xml_diff>